<commit_message>
work done on final report;
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d00bdda856596453/Documents/ScientificComputing/Dakota-Dalton-Sci-Comp-Project/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dakota\OneDrive\Documents\ScientificComputing\Dakota-Dalton-Sci-Comp-Project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
   <si>
     <t>Laplace</t>
-  </si>
-  <si>
-    <t>delta</t>
   </si>
   <si>
     <t>max</t>
@@ -46,18 +43,44 @@
   <si>
     <t>Poisson</t>
   </si>
+  <si>
+    <t>Helmholtz</t>
+  </si>
+  <si>
+    <t>Gauss-Seidel</t>
+  </si>
+  <si>
+    <t># nodes</t>
+  </si>
+  <si>
+    <t>Δ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,21 +91,242 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -365,127 +609,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J10"/>
+  <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="L3" s="18"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="Q4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="R4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>11.6244</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-25.044</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-122.9058</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="H3">
-        <v>11.6244</v>
-      </c>
-      <c r="I3">
-        <v>-24.960899999999999</v>
-      </c>
-      <c r="J3">
-        <v>-122.9058</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K5" s="7">
         <v>0.25</v>
       </c>
-      <c r="C4" s="1">
+      <c r="L5" s="4">
+        <v>632</v>
+      </c>
+      <c r="M5" s="8">
         <v>11.538399999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="N5" s="8">
         <v>-25.314299999999999</v>
       </c>
-      <c r="E4" s="1">
+      <c r="O5" s="4">
         <v>-123.57859999999999</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="P5" s="8">
         <v>11.538399999999999</v>
       </c>
-      <c r="I4" s="1">
+      <c r="Q5" s="8">
         <v>-24.9498</v>
       </c>
-      <c r="J4" s="1">
+      <c r="R5" s="9">
         <v>-123.57859999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>11.636900000000001</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-24.8688</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-123.91500000000001</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>11.636900000000001</v>
-      </c>
-      <c r="I5" s="1">
-        <v>-24.495999999999999</v>
-      </c>
-      <c r="J5" s="1">
-        <v>-123.91500000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -494,113 +698,354 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="K6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3948</v>
+      </c>
+      <c r="M6" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="N6" s="8">
+        <v>-25.044</v>
+      </c>
+      <c r="O6" s="4">
+        <v>-122.9058</v>
+      </c>
+      <c r="P6" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>-24.960899999999999</v>
+      </c>
+      <c r="R6" s="9">
+        <v>-122.9058</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="K7" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L7" s="11">
+        <v>63165</v>
+      </c>
+      <c r="M7" s="12">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="N7" s="12">
+        <v>-24.8688</v>
+      </c>
+      <c r="O7" s="11">
+        <v>-123.91500000000001</v>
+      </c>
+      <c r="P7" s="12">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>-24.495999999999999</v>
+      </c>
+      <c r="R7" s="13">
+        <v>-123.91500000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="4">
+        <v>632</v>
+      </c>
+      <c r="D9" s="8">
+        <v>11.538399999999999</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-24.226800000000001</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-123.578</v>
+      </c>
+      <c r="G9" s="8">
+        <v>11.538399999999999</v>
+      </c>
+      <c r="H9" s="8">
+        <v>-24.9498</v>
+      </c>
+      <c r="I9" s="9">
+        <v>-123.57859999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3948</v>
+      </c>
+      <c r="D10" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="E10" s="8">
+        <v>-23.807400000000001</v>
+      </c>
+      <c r="F10" s="4">
+        <v>-122.9058</v>
+      </c>
+      <c r="G10" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="H10" s="8">
+        <v>-24.960899999999999</v>
+      </c>
+      <c r="I10" s="9">
+        <v>-122.9058</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C11" s="11">
+        <v>63165</v>
+      </c>
+      <c r="D11" s="12">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="E11" s="12">
+        <v>-23.699200000000001</v>
+      </c>
+      <c r="F11" s="11">
+        <v>-123.91500000000001</v>
+      </c>
+      <c r="G11" s="12">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="H11" s="12">
+        <v>-24.495999999999999</v>
+      </c>
+      <c r="I11" s="13">
+        <v>-123.91500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C8">
-        <v>11.538399999999999</v>
-      </c>
-      <c r="D8">
-        <v>-24.226800000000001</v>
-      </c>
-      <c r="E8">
-        <v>-123.578</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="H8">
-        <v>11.538399999999999</v>
-      </c>
-      <c r="I8">
-        <v>-24.9498</v>
-      </c>
-      <c r="J8">
-        <v>-123.57859999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1755</v>
+      </c>
+      <c r="D17" s="8">
+        <v>11.6076</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-383.61430000000001</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-761.4203</v>
+      </c>
+      <c r="G17" s="8">
+        <v>11.6076</v>
+      </c>
+      <c r="H17" s="8">
+        <v>-2188.6</v>
+      </c>
+      <c r="I17" s="9">
+        <v>-5195.3999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
         <v>0.1</v>
       </c>
-      <c r="C9">
+      <c r="C18" s="4">
+        <v>3948</v>
+      </c>
+      <c r="D18" s="8">
         <v>11.6244</v>
       </c>
-      <c r="D9">
-        <v>-23.807400000000001</v>
-      </c>
-      <c r="E9">
-        <v>-122.9058</v>
-      </c>
-      <c r="H9">
+      <c r="E18" s="8">
+        <v>-170.72120000000001</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-372.0874</v>
+      </c>
+      <c r="G18" s="8">
         <v>11.6244</v>
       </c>
-      <c r="I9">
-        <v>-24.960899999999999</v>
-      </c>
-      <c r="J9">
-        <v>-122.9058</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+      <c r="H18" s="8">
+        <v>-224.16669999999999</v>
+      </c>
+      <c r="I18" s="9">
+        <v>-462.0643</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="4">
+        <v>15791</v>
+      </c>
+      <c r="D19" s="8">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="E19" s="8">
+        <v>-259.2955</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-534.75459999999998</v>
+      </c>
+      <c r="G19" s="8">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="H19" s="8">
+        <v>-276.69589999999999</v>
+      </c>
+      <c r="I19" s="9">
+        <v>-560.35429999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C10">
+      <c r="C20" s="19">
+        <v>63165</v>
+      </c>
+      <c r="D20" s="8">
         <v>11.636900000000001</v>
       </c>
-      <c r="D10">
-        <v>-23.699200000000001</v>
-      </c>
-      <c r="E10">
-        <v>-123.91500000000001</v>
-      </c>
-      <c r="H10">
+      <c r="E20" s="8">
+        <v>-514.54949999999997</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-1004.4</v>
+      </c>
+      <c r="G20" s="8">
         <v>11.636900000000001</v>
       </c>
-      <c r="I10">
-        <v>-24.495999999999999</v>
-      </c>
-      <c r="J10">
-        <v>-123.91500000000001</v>
+      <c r="H20" s="8">
+        <v>-526.9597</v>
+      </c>
+      <c r="I20" s="9">
+        <v>-1023.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="21">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="C21" s="11">
+        <v>252662</v>
+      </c>
+      <c r="D21" s="12">
+        <v>11.6378</v>
+      </c>
+      <c r="E21" s="12">
+        <v>-503.86829999999998</v>
+      </c>
+      <c r="F21" s="11">
+        <v>-982.95550000000003</v>
+      </c>
+      <c r="G21" s="12">
+        <v>11.6378</v>
+      </c>
+      <c r="H21" s="12">
+        <v>-242.32769999999999</v>
+      </c>
+      <c r="I21" s="13">
+        <v>-500.0822</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
just about finished final report;
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
   <si>
     <t>Laplace</t>
   </si>
@@ -55,12 +55,60 @@
   <si>
     <t>Δ</t>
   </si>
+  <si>
+    <t># iterations</t>
+  </si>
+  <si>
+    <r>
+      <t>SOR (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>λ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1.2)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOR λ</t>
+  </si>
+  <si>
+    <t>Δ = 0.025</t>
+  </si>
+  <si>
+    <r>
+      <t>Helmholtz (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Λ = -1)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +130,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -260,11 +315,203 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,19 +561,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,23 +967,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R21"/>
+  <dimension ref="B2:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K3" s="17" t="s">
+    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="18"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14" t="s">
         <v>7</v>
@@ -637,7 +996,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K4" s="5" t="s">
         <v>9</v>
       </c>
@@ -663,7 +1022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K5" s="7">
         <v>0.25</v>
       </c>
@@ -689,7 +1048,7 @@
         <v>-123.57859999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -723,11 +1082,11 @@
         <v>-122.9058</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
         <v>7</v>
@@ -763,7 +1122,7 @@
         <v>-123.91500000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -789,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>0.25</v>
       </c>
@@ -815,7 +1174,7 @@
         <v>-123.57859999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>0.1</v>
       </c>
@@ -841,7 +1200,7 @@
         <v>-122.9058</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -867,12 +1226,46 @@
         <v>-123.91500000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
+    <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L13" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="56"/>
+      <c r="P13" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="52"/>
+      <c r="P14" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="40"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
         <v>7</v>
@@ -883,8 +1276,24 @@
         <v>4</v>
       </c>
       <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>3948</v>
+      </c>
+      <c r="N15" s="41">
+        <v>964</v>
+      </c>
+      <c r="O15" s="42"/>
+      <c r="P15" s="41">
+        <v>682</v>
+      </c>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
@@ -909,8 +1318,24 @@
       <c r="I16" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="M16" s="4">
+        <v>15791</v>
+      </c>
+      <c r="N16" s="43">
+        <v>4421</v>
+      </c>
+      <c r="O16" s="44"/>
+      <c r="P16" s="43">
+        <v>2923</v>
+      </c>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>0.15</v>
       </c>
@@ -935,8 +1360,24 @@
       <c r="I17" s="9">
         <v>-5195.3999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L17" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M17" s="17">
+        <v>63165</v>
+      </c>
+      <c r="N17" s="43">
+        <v>21210</v>
+      </c>
+      <c r="O17" s="44"/>
+      <c r="P17" s="43">
+        <v>13903</v>
+      </c>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>0.1</v>
       </c>
@@ -961,8 +1402,24 @@
       <c r="I18" s="9">
         <v>-462.0643</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L18" s="19">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="M18" s="11">
+        <v>252662</v>
+      </c>
+      <c r="N18" s="45">
+        <v>84503</v>
+      </c>
+      <c r="O18" s="46"/>
+      <c r="P18" s="49">
+        <v>45094</v>
+      </c>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>0.05</v>
       </c>
@@ -987,12 +1444,14 @@
       <c r="I19" s="9">
         <v>-560.35429999999997</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="20">
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="17">
         <v>63165</v>
       </c>
       <c r="D20" s="8">
@@ -1013,9 +1472,11 @@
       <c r="I20" s="9">
         <v>-1023.5</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="21">
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+    </row>
+    <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="19">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="C21" s="11">
@@ -1039,12 +1500,258 @@
       <c r="I21" s="13">
         <v>-500.0822</v>
       </c>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+    </row>
+    <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="M23" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="38"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C25" s="23">
+        <v>3948</v>
+      </c>
+      <c r="D25" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="E25" s="8">
+        <v>-12.568199999999999</v>
+      </c>
+      <c r="F25" s="23">
+        <v>-122.9058</v>
+      </c>
+      <c r="G25" s="8">
+        <v>11.6244</v>
+      </c>
+      <c r="H25" s="8">
+        <v>-12.8613</v>
+      </c>
+      <c r="I25" s="26">
+        <v>-122.9058</v>
+      </c>
+      <c r="M25" s="29">
+        <v>1</v>
+      </c>
+      <c r="N25" s="30">
+        <v>17183</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C26" s="24">
+        <v>63165</v>
+      </c>
+      <c r="D26" s="22">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="E26" s="22">
+        <v>-12.152100000000001</v>
+      </c>
+      <c r="F26" s="24">
+        <v>-123.91500000000001</v>
+      </c>
+      <c r="G26" s="22">
+        <v>11.636900000000001</v>
+      </c>
+      <c r="H26" s="22">
+        <v>-12.447100000000001</v>
+      </c>
+      <c r="I26" s="27">
+        <v>-123.91500000000001</v>
+      </c>
+      <c r="M26" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N26" s="4">
+        <v>14078</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="M27" s="31">
+        <v>1.2</v>
+      </c>
+      <c r="N27" s="4">
+        <v>13903</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="M28" s="31">
+        <v>1.3</v>
+      </c>
+      <c r="N28" s="4">
+        <v>11255</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="36"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="M29" s="31">
+        <v>1.4</v>
+      </c>
+      <c r="N29" s="4">
+        <v>8985</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="M30" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="N30" s="4">
+        <v>7019</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="M31" s="31">
+        <v>1.6</v>
+      </c>
+      <c r="N31" s="4">
+        <v>5299</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M32" s="31">
+        <v>1.7</v>
+      </c>
+      <c r="N32" s="4">
+        <v>3783</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M33" s="31">
+        <v>1.8</v>
+      </c>
+      <c r="N33" s="4">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M34" s="31">
+        <v>1.9</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="32">
+        <v>2</v>
+      </c>
+      <c r="N35" s="3">
+        <v>24280</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="18">
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>